<commit_message>
Work for 2023-0112, which concerned troubleshooting the Singularity mount/data-access issue and then refactoring, testing, and running code for Trinity GF jobs; also, spent a good bit of time designing the Trinity optimization experiment (see the .xlsx file)
</commit_message>
<xml_diff>
--- a/results/2022-1101/notebook/trinity-parameters.xlsx
+++ b/results/2022-1101/notebook/trinity-parameters.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/homes/tsukiyamalab/kalavatt/2022_transcriptome-construction/results/2022-1101/notebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavatt/projects-etc/2022_transcriptome-construction/results/2022-1101/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8436491-EA12-C74A-BF0E-10AA99FF03C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21706EE-FDA1-154C-9860-424AAFEE9458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="7700" windowWidth="38400" windowHeight="21100" xr2:uid="{8F9F2F58-FFA3-AE48-BF61-DF943E6DC9C3}"/>
+    <workbookView xWindow="51200" yWindow="7700" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{8F9F2F58-FFA3-AE48-BF61-DF943E6DC9C3}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
-    <sheet name="draft" sheetId="2" r:id="rId2"/>
+    <sheet name="draft_2022-1201" sheetId="2" r:id="rId2"/>
+    <sheet name="draft_2023-0111_draft" sheetId="3" r:id="rId3"/>
+    <sheet name="draft_2023-0111_succinct" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="154">
   <si>
     <t>parameter</t>
   </si>
@@ -156,9 +158,6 @@
     <t>"--min_iso_ratio just takes the kmer abundance into account when doing the inchworm contig clustering, mainly to prevent very lowly expressed contigs from being clustered together with highly expressed contigs"</t>
   </si>
   <si>
-    <t>0.01, 0.05, #TBD</t>
-  </si>
-  <si>
     <t>--glue_factor</t>
   </si>
   <si>
@@ -171,9 +170,6 @@
     <t>--normalize_max_read_cov</t>
   </si>
   <si>
-    <t>"It means that 'poorly covered regions are unchanged, but reads are down-sampled in high-coverage regions (see slide 16 at link)"</t>
-  </si>
-  <si>
     <t>biohpc.cornell.edu/lab/doc/Trinity_workshop.pdf</t>
   </si>
   <si>
@@ -192,9 +188,6 @@
     <t>option</t>
   </si>
   <si>
-    <t>#NOTE Necessary for us; using --jaccard_clip is recommended for small-genome organisms such as fungi</t>
-  </si>
-  <si>
     <t>--output</t>
   </si>
   <si>
@@ -259,9 +252,6 @@
   </si>
   <si>
     <t>No default value, but this must be specified if performing genome-guided assenbly (see line 1211 of source code)</t>
-  </si>
-  <si>
-    <t>25, 50, 100, 200</t>
   </si>
   <si>
     <t>specified_Alison</t>
@@ -455,12 +445,302 @@
   <si>
     <t>"\${f_guided}"</t>
   </si>
+  <si>
+    <t>"It means that 'poorly covered regions are unchanged, but reads are down-sampled in high-coverage regions"</t>
+  </si>
+  <si>
+    <t>(see slide 16)</t>
+  </si>
+  <si>
+    <t>#NOTE Necessary for us: Using --jaccard_clip is recommended for small-genome organisms such as fungi</t>
+  </si>
+  <si>
+    <t>(see slide 17)</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>link to informative Trinity forum post</t>
+  </si>
+  <si>
+    <t>10, 25, 50, 100, 200</t>
+  </si>
+  <si>
+    <t>0.005, 0.01, 0.05, 0.1</t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>value_2022-1201</t>
+  </si>
+  <si>
+    <t>1, 2, 4, 8, 16, 32, 64, 128, 256, 512</t>
+  </si>
+  <si>
+    <t>\${SLURM_CPUS_ON_NODE}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (product)</t>
+    </r>
+  </si>
+  <si>
+    <t>command_genome-guided</t>
+  </si>
+  <si>
+    <t>command_genome-free</t>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>, everything</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>, McIlwain et al.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>, McIlwain et al. with addition (--glue_factor)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>, McIlwain et al. with addition (--glue_factor, --min_iso_ratio)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>, PASA conditions: 3 (product)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>, PASA conditions: 5 (product)</t>
+    </r>
+  </si>
+  <si>
+    <t>PASA conditions: 3</t>
+  </si>
+  <si>
+    <t>--gene_overlap</t>
+  </si>
+  <si>
+    <t>--stringent_alignment_overlap</t>
+  </si>
+  <si>
+    <t>#DEFAULT (minimal_overlap)</t>
+  </si>
+  <si>
+    <t>preference</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>PASA conditions: 5</t>
+  </si>
+  <si>
+    <t>developers</t>
+  </si>
+  <si>
+    <t>PASA setup</t>
+  </si>
+  <si>
+    <t>0.01, 0.05</t>
+  </si>
+  <si>
+    <t>How many datasets when its all said and done?</t>
+  </si>
+  <si>
+    <t>What are the PASA conditions that will be varied?</t>
+  </si>
+  <si>
+    <t>#CONTEXTUAL</t>
+  </si>
+  <si>
+    <t>When finished, how many datasets?</t>
+  </si>
+  <si>
+    <t>tally</t>
+  </si>
+  <si>
+    <t>PASA</t>
+  </si>
+  <si>
+    <t>Trinity</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">program (i.e., </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>after having run it</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>conditions: 5</t>
+  </si>
+  <si>
+    <t>Trinity parameter</t>
+  </si>
+  <si>
+    <t>PASA parameter</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trinity experimental conditions for experiments associated with directories </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>results/{2022-1201,2023-0111}/</t>
+    </r>
+  </si>
+  <si>
+    <t>values_2023-0111</t>
+  </si>
+  <si>
+    <t>values_2023-0111 (final decision)</t>
+  </si>
+  <si>
+    <t>values_2023-0111 (everything)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -542,12 +822,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Consolas"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FFFF9814"/>
       <name val="Consolas"/>
       <family val="2"/>
@@ -564,8 +838,35 @@
       <name val="Consolas"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FFFF9814"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -584,8 +885,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -632,12 +945,104 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -660,34 +1065,127 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -697,9 +1195,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDBFFC5"/>
       <color rgb="FFFF9814"/>
       <color rgb="FFEAFFE0"/>
-      <color rgb="FFDBFFC5"/>
       <color rgb="FFD8FBFF"/>
     </mruColors>
   </colors>
@@ -1013,7 +1511,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B65B96-9B80-CF46-9873-F5744C4478B7}">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1029,13 +1529,13 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -1044,16 +1544,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
@@ -1062,9 +1562,9 @@
         <v>4</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -1086,13 +1586,13 @@
         <v>10</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>12</v>
@@ -1105,7 +1605,7 @@
       <c r="B2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -1117,25 +1617,25 @@
       <c r="F2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>23</v>
       </c>
       <c r="H2" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J2" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="M2" s="17" t="s">
         <v>24</v>
       </c>
       <c r="N2" s="3" t="e">
@@ -1164,8 +1664,8 @@
       <c r="B3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>108</v>
+      <c r="C3" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>18</v>
@@ -1176,25 +1676,25 @@
       <c r="F3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="20">
         <v>6</v>
       </c>
       <c r="H3" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J3" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="17">
         <v>2</v>
       </c>
       <c r="N3" s="3" t="e">
@@ -1223,7 +1723,7 @@
       <c r="B4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -1235,25 +1735,25 @@
       <c r="F4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="20" t="s">
         <v>15</v>
       </c>
       <c r="H4" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J4" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="M4" s="18" t="e">
+      <c r="M4" s="17" t="e">
         <v>#N/A</v>
       </c>
       <c r="N4" s="3" t="e">
@@ -1266,7 +1766,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>17</v>
@@ -1283,10 +1783,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>14</v>
@@ -1294,14 +1794,14 @@
       <c r="F5" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G5" s="22" t="s">
-        <v>47</v>
+      <c r="G5" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="H5" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J5" s="7" t="b">
         <v>0</v>
@@ -1312,20 +1812,20 @@
       <c r="L5" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M5" s="19" t="e">
+      <c r="M5" s="18" t="e">
         <v>#N/A</v>
       </c>
       <c r="N5" s="8" t="e">
         <v>#N/A</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="P5" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="W5" s="1" t="e">
         <v>#N/A</v>
@@ -1338,11 +1838,11 @@
       <c r="B6" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>105</v>
+      <c r="C6" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>19</v>
@@ -1350,7 +1850,7 @@
       <c r="F6" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="21">
         <v>1002</v>
       </c>
       <c r="H6" s="7" t="b">
@@ -1368,35 +1868,35 @@
       <c r="L6" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M6" s="19" t="e">
+      <c r="M6" s="18" t="e">
         <v>#N/A</v>
       </c>
       <c r="N6" s="8" t="e">
         <v>#N/A</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="P6" s="15" t="s">
-        <v>101</v>
+        <v>84</v>
+      </c>
+      <c r="P6" s="28" t="s">
+        <v>97</v>
       </c>
       <c r="Q6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="R6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="U6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V6" s="14" t="s">
-        <v>98</v>
+        <v>70</v>
+      </c>
+      <c r="V6" s="27" t="s">
+        <v>94</v>
       </c>
       <c r="W6" s="1" t="e">
         <v>#N/A</v>
@@ -1409,26 +1909,26 @@
       <c r="B7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>49</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F7" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="21" t="s">
-        <v>47</v>
+      <c r="G7" s="20" t="s">
+        <v>45</v>
       </c>
       <c r="H7" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J7" s="1" t="b">
         <v>0</v>
@@ -1439,7 +1939,7 @@
       <c r="L7" s="1" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M7" s="18" t="e">
+      <c r="M7" s="17" t="e">
         <v>#N/A</v>
       </c>
       <c r="N7" s="3" t="e">
@@ -1452,10 +1952,16 @@
         <v>#N/A</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>51</v>
+        <v>110</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="W7" s="1" t="e">
         <v>#N/A</v>
@@ -1469,10 +1975,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>14</v>
@@ -1480,25 +1986,25 @@
       <c r="F8" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G8" s="21" t="s">
-        <v>47</v>
+      <c r="G8" s="20" t="s">
+        <v>45</v>
       </c>
       <c r="H8" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J8" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L8" s="1" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M8" s="18" t="e">
+      <c r="M8" s="17" t="e">
         <v>#N/A</v>
       </c>
       <c r="N8" s="3" t="e">
@@ -1511,7 +2017,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="W8" s="1" t="e">
         <v>#N/A</v>
@@ -1524,26 +2030,26 @@
       <c r="B9" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>47</v>
+      <c r="C9" s="15" t="s">
+        <v>45</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F9" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G9" s="21" t="s">
-        <v>47</v>
+      <c r="G9" s="20" t="s">
+        <v>45</v>
       </c>
       <c r="H9" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J9" s="4" t="e">
         <v>#N/A</v>
@@ -1554,7 +2060,7 @@
       <c r="L9" s="1" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M9" s="18" t="e">
+      <c r="M9" s="17" t="e">
         <v>#N/A</v>
       </c>
       <c r="N9" s="3" t="e">
@@ -1567,7 +2073,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="W9" s="1" t="e">
         <v>#N/A</v>
@@ -1580,7 +2086,7 @@
       <c r="B10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <v>1</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -1592,7 +2098,7 @@
       <c r="F10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="20">
         <v>2</v>
       </c>
       <c r="H10" s="1" t="b">
@@ -1610,7 +2116,7 @@
       <c r="L10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="17">
         <v>1</v>
       </c>
       <c r="N10" s="3">
@@ -1619,7 +2125,7 @@
       <c r="O10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P10" s="15" t="s">
+      <c r="P10" s="14" t="s">
         <v>32</v>
       </c>
       <c r="Q10" s="1" t="s">
@@ -1639,7 +2145,7 @@
       <c r="B11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <v>0.05</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1651,14 +2157,14 @@
       <c r="F11" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G11" s="21" t="s">
-        <v>71</v>
+      <c r="G11" s="20" t="s">
+        <v>68</v>
       </c>
       <c r="H11" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J11" s="1" t="b">
         <v>1</v>
@@ -1669,7 +2175,7 @@
       <c r="L11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="17">
         <v>0.05</v>
       </c>
       <c r="N11" s="3">
@@ -1678,12 +2184,15 @@
       <c r="O11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P11" s="15" t="s">
-        <v>39</v>
+      <c r="P11" s="14" t="s">
+        <v>115</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="R11" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="W11" s="1" t="e">
         <v>#N/A</v>
       </c>
@@ -1707,7 +2216,7 @@
       <c r="F12" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="20">
         <v>2</v>
       </c>
       <c r="H12" s="1" t="b">
@@ -1725,21 +2234,24 @@
       <c r="L12" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="17">
         <v>2</v>
       </c>
       <c r="N12" s="3">
         <v>3</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P12" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" s="14" t="s">
         <v>35</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="R12" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="W12" s="1" t="e">
         <v>#N/A</v>
       </c>
@@ -1751,11 +2263,11 @@
       <c r="B13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="17">
         <v>0.05</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>37</v>
@@ -1763,14 +2275,14 @@
       <c r="F13" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G13" s="21" t="s">
-        <v>71</v>
+      <c r="G13" s="20" t="s">
+        <v>68</v>
       </c>
       <c r="H13" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J13" s="1" t="b">
         <v>1</v>
@@ -1781,20 +2293,23 @@
       <c r="L13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="17">
         <v>0.05</v>
       </c>
       <c r="N13" s="3">
         <v>3</v>
       </c>
       <c r="O13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P13" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>42</v>
+      <c r="R13" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="W13" s="1" t="e">
         <v>#N/A</v>
@@ -1807,11 +2322,11 @@
       <c r="B14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="17">
         <v>200000</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>19</v>
@@ -1819,38 +2334,38 @@
       <c r="F14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="20">
         <v>500000</v>
       </c>
       <c r="H14" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J14" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L14" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="17">
         <v>200000</v>
       </c>
       <c r="N14" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P14" s="15" t="s">
-        <v>101</v>
+        <v>40</v>
+      </c>
+      <c r="P14" s="28" t="s">
+        <v>97</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="W14" s="1" t="e">
         <v>#N/A</v>
@@ -1863,11 +2378,11 @@
       <c r="B15" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="17">
         <v>200</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>19</v>
@@ -1875,7 +2390,7 @@
       <c r="F15" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="20">
         <v>200</v>
       </c>
       <c r="H15" s="3" t="b">
@@ -1893,23 +2408,26 @@
       <c r="L15" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="M15" s="18">
+      <c r="M15" s="17">
         <v>200</v>
       </c>
       <c r="N15" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="P15" s="15" t="s">
-        <v>74</v>
+        <v>82</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>114</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="W15" s="1" t="e">
         <v>#N/A</v>
@@ -1922,11 +2440,11 @@
       <c r="B16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="15">
         <v>700</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>19</v>
@@ -1934,7 +2452,7 @@
       <c r="F16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="20">
         <v>700</v>
       </c>
       <c r="H16" s="1" t="b">
@@ -1947,25 +2465,25 @@
         <v>0</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L16" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="M16" s="18">
+      <c r="M16" s="17">
         <v>500</v>
       </c>
       <c r="N16" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P16" s="15" t="s">
-        <v>101</v>
+        <v>61</v>
+      </c>
+      <c r="P16" s="28" t="s">
+        <v>97</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="W16" s="1" t="e">
         <v>#N/A</v>
@@ -1978,11 +2496,11 @@
       <c r="B17" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="17">
         <v>200</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>19</v>
@@ -1990,7 +2508,7 @@
       <c r="F17" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="20">
         <v>200</v>
       </c>
       <c r="H17" s="1" t="b">
@@ -2003,12 +2521,12 @@
         <v>0</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L17" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="M17" s="18">
+      <c r="M17" s="17">
         <v>200</v>
       </c>
       <c r="N17" s="3" t="e">
@@ -2021,10 +2539,10 @@
         <v>#N/A</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="W17" s="1" t="e">
         <v>#N/A</v>
@@ -2038,10 +2556,10 @@
         <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>14</v>
@@ -2049,7 +2567,7 @@
       <c r="F18" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G18" s="23" t="e">
+      <c r="G18" s="22" t="e">
         <v>#N/A</v>
       </c>
       <c r="H18" s="12" t="e">
@@ -2062,25 +2580,25 @@
         <v>1</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L18" s="13" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M18" s="20" t="e">
+      <c r="M18" s="19" t="e">
         <v>#N/A</v>
       </c>
       <c r="N18" s="13" t="e">
         <v>#N/A</v>
       </c>
       <c r="O18" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="P18" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="W18" s="1" t="e">
         <v>#N/A</v>
@@ -2094,10 +2612,10 @@
         <v>0</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>14</v>
@@ -2105,7 +2623,7 @@
       <c r="F19" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G19" s="23" t="e">
+      <c r="G19" s="22" t="e">
         <v>#N/A</v>
       </c>
       <c r="H19" s="12" t="e">
@@ -2118,25 +2636,25 @@
         <v>1</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L19" s="13" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M19" s="20" t="e">
+      <c r="M19" s="19" t="e">
         <v>#N/A</v>
       </c>
       <c r="N19" s="13" t="e">
         <v>#N/A</v>
       </c>
       <c r="O19" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="P19" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="W19" s="1" t="e">
         <v>#N/A</v>
@@ -2150,10 +2668,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>14</v>
@@ -2161,7 +2679,7 @@
       <c r="F20" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G20" s="23" t="e">
+      <c r="G20" s="22" t="e">
         <v>#N/A</v>
       </c>
       <c r="H20" s="12" t="e">
@@ -2174,25 +2692,25 @@
         <v>1</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L20" s="13" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M20" s="20" t="e">
+      <c r="M20" s="19" t="e">
         <v>#N/A</v>
       </c>
       <c r="N20" s="13" t="e">
         <v>#N/A</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="P20" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="W20" s="1" t="e">
         <v>#N/A</v>
@@ -2206,8 +2724,8 @@
         <v>0</v>
       </c>
       <c r="C21" s="6"/>
-      <c r="D21" s="25" t="s">
-        <v>81</v>
+      <c r="D21" s="24" t="s">
+        <v>77</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>14</v>
@@ -2215,7 +2733,7 @@
       <c r="F21" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G21" s="26" t="e">
+      <c r="G21" s="25" t="e">
         <v>#N/A</v>
       </c>
       <c r="H21" s="5" t="e">
@@ -2246,7 +2764,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q21" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
@@ -2265,16 +2783,16 @@
         <v>0</v>
       </c>
       <c r="C22" s="6"/>
-      <c r="D22" s="25" t="s">
-        <v>89</v>
+      <c r="D22" s="24" t="s">
+        <v>85</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F22" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G22" s="26" t="e">
+      <c r="G22" s="25" t="e">
         <v>#N/A</v>
       </c>
       <c r="H22" s="5" t="b">
@@ -2305,7 +2823,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
@@ -2324,8 +2842,8 @@
         <v>0</v>
       </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="25" t="s">
-        <v>90</v>
+      <c r="D23" s="24" t="s">
+        <v>86</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>14</v>
@@ -2333,7 +2851,7 @@
       <c r="F23" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G23" s="27" t="e">
+      <c r="G23" s="26" t="e">
         <v>#N/A</v>
       </c>
       <c r="H23" s="5" t="b">
@@ -2358,19 +2876,19 @@
         <v>#N/A</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="P23" s="6" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="S23" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="R23" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="S23" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
@@ -2383,39 +2901,43 @@
   <hyperlinks>
     <hyperlink ref="R15" r:id="rId1" display="https://biohpc.cornell.edu/lab/doc/Trinity_workshop.pdf" xr:uid="{315B092E-C843-8644-97BE-0BBE8892AF7B}"/>
     <hyperlink ref="S6" r:id="rId2" display="https://github.com/trinityrnaseq/trinityrnaseq/wiki/Genome-Guided-Trinity-Transcriptome-Assembly" xr:uid="{492CA23A-CF22-6B40-A03C-30B2F90B8258}"/>
+    <hyperlink ref="R11" r:id="rId3" display="link" xr:uid="{229F54C1-5B0B-644A-BEAD-113A7F515017}"/>
+    <hyperlink ref="S7" r:id="rId4" display="https://biohpc.cornell.edu/lab/doc/Trinity_workshop.pdf" xr:uid="{46929B5C-8904-BC40-8514-365667718CE4}"/>
+    <hyperlink ref="R12" r:id="rId5" display="link" xr:uid="{B2A0B857-FF7A-E34B-B204-C8663745A178}"/>
+    <hyperlink ref="R13" r:id="rId6" display="link" xr:uid="{053DA288-C0E6-F341-A68D-2CCA319A6C4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="P12" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A025907F-6809-5545-9D7D-A242F24C6350}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C6"/>
-    </sheetView>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="3" max="4" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>22</v>
+      <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2425,11 +2947,11 @@
       <c r="B2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>18</v>
+      <c r="C2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2439,11 +2961,11 @@
       <c r="B3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>13</v>
+      <c r="C3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2451,13 +2973,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>78</v>
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2467,11 +2989,11 @@
       <c r="B5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>79</v>
+      <c r="C5" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2481,11 +3003,11 @@
       <c r="B6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>80</v>
+      <c r="C6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2493,13 +3015,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>58</v>
+        <v>0</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2509,11 +3031,11 @@
       <c r="B8" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>49</v>
+      <c r="C8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2523,11 +3045,11 @@
       <c r="B9" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>52</v>
+      <c r="C9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2537,11 +3059,11 @@
       <c r="B10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>54</v>
+      <c r="C10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2551,11 +3073,11 @@
       <c r="B11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C11" s="18">
-        <v>1</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>28</v>
+      <c r="C11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2565,11 +3087,11 @@
       <c r="B12" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C12" s="18">
-        <v>0.05</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>36</v>
+      <c r="C12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2579,11 +3101,11 @@
       <c r="B13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C13" s="3">
-        <v>2</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>33</v>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0.05</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2593,11 +3115,11 @@
       <c r="B14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C14" s="18">
-        <v>0.05</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>40</v>
+      <c r="C14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2607,11 +3129,11 @@
       <c r="B15" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C15" s="18">
-        <v>200000</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>56</v>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="17">
+        <v>0.05</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2621,11 +3143,11 @@
       <c r="B16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="18">
-        <v>200</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>43</v>
+      <c r="C16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="17">
+        <v>200000</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2635,11 +3157,11 @@
       <c r="B17" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C17" s="16">
-        <v>700</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>63</v>
+      <c r="C17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="17">
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2649,14 +3171,1223 @@
       <c r="B18" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="15">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="17">
         <v>200</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{644013CB-DC31-A744-837E-B27655C4D55A}">
+  <dimension ref="A1:O42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+    <col min="13" max="13" width="40.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="3">
+        <v>1</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="M5" s="37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="M6" s="37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="M7" s="37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10" s="37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="3">
+        <v>1</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="17">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="3">
+        <v>10</v>
+      </c>
+      <c r="J12" s="1">
+        <v>10</v>
+      </c>
+      <c r="K12" s="1">
+        <v>10</v>
+      </c>
+      <c r="L12" s="1">
+        <v>10</v>
+      </c>
+      <c r="M12" s="38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="3">
+        <v>4</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1">
+        <v>2</v>
+      </c>
+      <c r="M13" s="38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I14" s="3">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1">
+        <v>3</v>
+      </c>
+      <c r="K14" s="1">
+        <v>3</v>
+      </c>
+      <c r="L14" s="1">
+        <v>3</v>
+      </c>
+      <c r="M14" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15" s="3">
+        <v>4</v>
+      </c>
+      <c r="J15" s="1">
+        <v>3</v>
+      </c>
+      <c r="K15" s="1">
+        <v>4</v>
+      </c>
+      <c r="L15" s="1">
+        <v>4</v>
+      </c>
+      <c r="M15" s="38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="17">
+        <v>200000</v>
+      </c>
+      <c r="E16" s="17">
+        <v>200000</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="3">
+        <v>1</v>
+      </c>
+      <c r="M16" s="39">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="17">
+        <v>200</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="3">
+        <v>5</v>
+      </c>
+      <c r="M17" s="39">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="15">
+        <v>700</v>
+      </c>
+      <c r="E18" s="15">
+        <v>700</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="M18" s="20">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="17">
+        <v>200</v>
+      </c>
+      <c r="E19" s="17">
+        <v>200</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="M19" s="40">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="3"/>
+      <c r="M20" s="17"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H21" s="41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H22" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="I22" s="30">
+        <f>PRODUCT(I2:I19)</f>
+        <v>2400</v>
+      </c>
+      <c r="J22" s="30">
+        <f>PRODUCT(J2:J19)</f>
+        <v>90</v>
+      </c>
+      <c r="K22" s="30">
+        <f>PRODUCT(K2:K19)</f>
+        <v>120</v>
+      </c>
+      <c r="L22" s="42">
+        <f>PRODUCT(L2:L19)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H23" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" s="32">
+        <f>3*I22</f>
+        <v>7200</v>
+      </c>
+      <c r="J23" s="32">
+        <f>3*J22</f>
+        <v>270</v>
+      </c>
+      <c r="K23" s="32">
+        <f>3*K22</f>
+        <v>360</v>
+      </c>
+      <c r="L23" s="43">
+        <f>3*L22</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H24" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="I24" s="33">
+        <f>5*I22</f>
+        <v>12000</v>
+      </c>
+      <c r="J24" s="33">
+        <f>5*J22</f>
+        <v>450</v>
+      </c>
+      <c r="K24" s="33">
+        <f>5*K22</f>
+        <v>600</v>
+      </c>
+      <c r="L24" s="44">
+        <f>5*L22</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L26" s="41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L27" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="M27" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="N27" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="O27" s="31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L28" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="M28" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="N28" s="46">
+        <v>30</v>
+      </c>
+      <c r="O28" s="47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L29" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="M29" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="N29" s="46">
+        <v>20</v>
+      </c>
+      <c r="O29" s="47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L30" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="M30" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="N30" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O30" s="47" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L31" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="M31" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="N31" s="51">
+        <v>30</v>
+      </c>
+      <c r="O31" s="47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L32" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="M32" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="N32" s="51">
+        <v>50</v>
+      </c>
+      <c r="O32" s="47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L33" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="M33" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="N33" s="51">
+        <v>20</v>
+      </c>
+      <c r="O33" s="47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L34" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="M34" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="N34" s="51">
+        <v>30</v>
+      </c>
+      <c r="O34" s="47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L35" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="M35" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="N35" s="52" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O35" s="50" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="9"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="9"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="9"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="9"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H15" r:id="rId1" display="link" xr:uid="{2BCC4BC5-8057-CE47-A7F7-B9CE92594F28}"/>
+    <hyperlink ref="H14" r:id="rId2" display="link" xr:uid="{DE9771F7-415A-F944-AAC3-4066D062496E}"/>
+    <hyperlink ref="H13" r:id="rId3" display="link" xr:uid="{25B7BA6E-DF53-7241-A82F-A0346F3122DC}"/>
+    <hyperlink ref="H17" r:id="rId4" display="https://biohpc.cornell.edu/lab/doc/Trinity_workshop.pdf" xr:uid="{884AC3C2-C04A-CC49-82E7-CD02390C736C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E14 M14" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A19AA3B-A7B0-864C-B5E4-F8D7A1F6D4E7}">
+  <dimension ref="B1:F33"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="35.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="54" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="57" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="57" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="56">
+        <v>1</v>
+      </c>
+      <c r="D13" s="60" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="56">
+        <v>0.05</v>
+      </c>
+      <c r="D14" s="60" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="56">
+        <v>2</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="56">
+        <v>0.05</v>
+      </c>
+      <c r="D16" s="60" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="56">
+        <v>200000</v>
+      </c>
+      <c r="D17" s="61">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="56">
+        <v>200</v>
+      </c>
+      <c r="D18" s="61">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="56">
+        <v>700</v>
+      </c>
+      <c r="D19" s="57">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="63">
+        <v>200</v>
+      </c>
+      <c r="D20" s="64">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="54"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="51">
+        <v>30</v>
+      </c>
+      <c r="F24" s="47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C25" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="51">
+        <v>50</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26" s="51">
+        <v>20</v>
+      </c>
+      <c r="F26" s="47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="D27" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="51">
+        <v>30</v>
+      </c>
+      <c r="F27" s="47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="D28" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" s="52" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F28" s="50" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="54"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C31" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" s="53" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C32" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" s="53">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C33" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D15" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Continued work with the job-array/list-of-parameter material, typing up and submitting questions to Brian (to be properly documented in 2023-0111/, including his answers and my responses), and roughly assessing the results of Trinity parameterization experiments from the Jan. 12-14 data range: Simple metrics, getting a sense of the numbers of transcripts in files, what jobs failed and for what reasons (e.g., insufficient k-mer coverage), etc.
</commit_message>
<xml_diff>
--- a/results/2022-1101/notebook/trinity-parameters.xlsx
+++ b/results/2022-1101/notebook/trinity-parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavatt/projects-etc/2022_transcriptome-construction/results/2022-1101/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040DEC83-8F9C-0646-A2F8-4AB610B1F73C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC87024-8CDD-F94F-A80C-96CE13FD31EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="3600" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{8F9F2F58-FFA3-AE48-BF61-DF943E6DC9C3}"/>
+    <workbookView xWindow="7620" yWindow="3600" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{8F9F2F58-FFA3-AE48-BF61-DF943E6DC9C3}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="164">
   <si>
     <t>parameter</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>values_to_test_potential_1</t>
-  </si>
-  <si>
-    <t>values_to_test_potential_2</t>
   </si>
   <si>
     <t>--SS_lib_type</t>
@@ -628,9 +625,6 @@
     </r>
   </si>
   <si>
-    <t>PASA conditions: 3</t>
-  </si>
-  <si>
     <t>--gene_overlap</t>
   </si>
   <si>
@@ -668,12 +662,6 @@
   </si>
   <si>
     <t>When finished, how many datasets?</t>
-  </si>
-  <si>
-    <t>PASA</t>
-  </si>
-  <si>
-    <t>Trinity</t>
   </si>
   <si>
     <r>
@@ -736,9 +724,6 @@
     <t>1, 2, 4, 8, 16, 32, 64</t>
   </si>
   <si>
-    <t>update_2023-0113 (final decision)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">values_2023-0111 </t>
     </r>
@@ -760,14 +745,92 @@
     <t>tally (2023-0113)</t>
   </si>
   <si>
-    <t>Trinity (considering GF, GG)</t>
+    <t>update_2023-0125</t>
+  </si>
+  <si>
+    <t>1, 2, 4, 8, 16</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">update_2023-0113 </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>(final decision)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>, conditions (PASA, 3; Trinity, 1): 4 (product)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>, conditions (PASA, 5; Trinity, 1): 6 (product)</t>
+    </r>
+  </si>
+  <si>
+    <t>PASA conditions: 3 (AG)</t>
+  </si>
+  <si>
+    <t>PASA conditions: 3 (developers)</t>
+  </si>
+  <si>
+    <t>1, 2, 4, 8, 16, 32</t>
+  </si>
+  <si>
+    <t>tally (A; 2023-0125)</t>
+  </si>
+  <si>
+    <t>tally (B; 2023-0125)</t>
+  </si>
+  <si>
+    <t>update_2023-0125 (A; final decision)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -892,8 +955,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -936,8 +1013,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1086,15 +1169,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFFF0000"/>
       </left>
@@ -1122,43 +1196,6 @@
       <top/>
       <bottom style="thin">
         <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1205,15 +1242,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -1245,12 +1273,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1379,7 +1459,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1390,76 +1470,117 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1783,10 +1904,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B65B96-9B80-CF46-9873-F5744C4478B7}">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1795,21 +1917,25 @@
     <col min="3" max="4" width="24.83203125" style="1" customWidth="1"/>
     <col min="5" max="14" width="12.83203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="12.83203125" style="1" customWidth="1"/>
-    <col min="21" max="22" width="10.83203125" style="1"/>
-    <col min="23" max="23" width="12.83203125" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="10.83203125" style="1"/>
+    <col min="16" max="16" width="12.83203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="255.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="118.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="255.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="64.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="105.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="76.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -1818,16 +1944,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
@@ -1836,7 +1962,7 @@
         <v>4</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M1" s="16" t="s">
         <v>5</v>
@@ -1860,19 +1986,16 @@
         <v>10</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="b">
         <v>1</v>
       </c>
@@ -1880,58 +2003,55 @@
         <v>1</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>23</v>
-      </c>
       <c r="H2" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J2" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L2" s="1" t="b">
         <v>0</v>
       </c>
       <c r="M2" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W2" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="b">
         <v>1</v>
       </c>
@@ -1939,13 +2059,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>1</v>
@@ -1957,13 +2077,13 @@
         <v>1</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J3" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L3" s="1" t="b">
         <v>0</v>
@@ -1975,22 +2095,19 @@
         <v>#N/A</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P3" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W3" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="b">
         <v>1</v>
       </c>
@@ -1998,31 +2115,31 @@
         <v>1</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>15</v>
-      </c>
       <c r="H4" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J4" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L4" s="1" t="b">
         <v>0</v>
@@ -2034,22 +2151,19 @@
         <v>#N/A</v>
       </c>
       <c r="O4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W4" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="b">
         <v>0</v>
       </c>
@@ -2057,25 +2171,25 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>45</v>
-      </c>
       <c r="H5" s="7" t="b">
         <v>1</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J5" s="7" t="b">
         <v>0</v>
@@ -2093,19 +2207,16 @@
         <v>#N/A</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P5" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="W5" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="b">
         <v>0</v>
       </c>
@@ -2113,13 +2224,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="7" t="b">
         <v>1</v>
@@ -2149,34 +2260,31 @@
         <v>#N/A</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P6" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="T6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="T6" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="U6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V6" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="W6" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="b">
         <v>1</v>
       </c>
@@ -2184,25 +2292,25 @@
         <v>1</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="F7" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H7" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J7" s="1" t="b">
         <v>0</v>
@@ -2220,28 +2328,25 @@
         <v>#N/A</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P7" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="S7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="W7" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="b">
         <v>1</v>
       </c>
@@ -2249,111 +2354,105 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M8" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N8" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P8" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M8" s="17" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N8" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P8" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="W8" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K9" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L9" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M9" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N9" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K9" s="4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L9" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M9" s="17" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N9" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P9" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="W9" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="b">
         <v>1</v>
       </c>
@@ -2364,10 +2463,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="1" t="b">
         <v>1</v>
@@ -2397,22 +2496,19 @@
         <v>10</v>
       </c>
       <c r="O10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P10" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="W10" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="b">
         <v>1</v>
       </c>
@@ -2423,22 +2519,22 @@
         <v>0.05</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="F11" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H11" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J11" s="1" t="b">
         <v>1</v>
@@ -2456,22 +2552,19 @@
         <v>3</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="W11" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="b">
         <v>1</v>
       </c>
@@ -2482,10 +2575,10 @@
         <v>2</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="1" t="b">
         <v>1</v>
@@ -2515,22 +2608,19 @@
         <v>3</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="W12" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="b">
         <v>1</v>
       </c>
@@ -2541,22 +2631,22 @@
         <v>0.05</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H13" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J13" s="1" t="b">
         <v>1</v>
@@ -2574,22 +2664,19 @@
         <v>3</v>
       </c>
       <c r="O13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P13" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="R13" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="W13" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="b">
         <v>1</v>
       </c>
@@ -2600,10 +2687,10 @@
         <v>200000</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="1" t="b">
         <v>1</v>
@@ -2615,13 +2702,13 @@
         <v>0</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J14" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L14" s="1" t="b">
         <v>0</v>
@@ -2633,19 +2720,16 @@
         <v>#N/A</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P14" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="W14" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="b">
         <v>1</v>
       </c>
@@ -2656,10 +2740,10 @@
         <v>200</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="1" t="b">
         <v>1</v>
@@ -2689,25 +2773,22 @@
         <v>#N/A</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P15" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S15" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="R15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="W15" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="b">
         <v>1</v>
       </c>
@@ -2718,10 +2799,10 @@
         <v>700</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16" s="1" t="b">
         <v>1</v>
@@ -2739,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L16" s="1" t="b">
         <v>0</v>
@@ -2751,19 +2832,16 @@
         <v>#N/A</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P16" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="W16" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="b">
         <v>1</v>
       </c>
@@ -2774,10 +2852,10 @@
         <v>200</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" s="1" t="b">
         <v>1</v>
@@ -2795,7 +2873,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L17" s="1" t="b">
         <v>0</v>
@@ -2807,22 +2885,19 @@
         <v>#N/A</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P17" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="W17" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="b">
         <v>1</v>
       </c>
@@ -2830,13 +2905,13 @@
         <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18" s="12" t="e">
         <v>#N/A</v>
@@ -2854,7 +2929,7 @@
         <v>1</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L18" s="13" t="e">
         <v>#N/A</v>
@@ -2866,19 +2941,16 @@
         <v>#N/A</v>
       </c>
       <c r="O18" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P18" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="W18" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="b">
         <v>1</v>
       </c>
@@ -2886,13 +2958,13 @@
         <v>0</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19" s="12" t="e">
         <v>#N/A</v>
@@ -2910,7 +2982,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L19" s="13" t="e">
         <v>#N/A</v>
@@ -2922,19 +2994,16 @@
         <v>#N/A</v>
       </c>
       <c r="O19" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P19" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="W19" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="b">
         <v>1</v>
       </c>
@@ -2942,13 +3011,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" s="12" t="e">
         <v>#N/A</v>
@@ -2966,7 +3035,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L20" s="13" t="e">
         <v>#N/A</v>
@@ -2978,19 +3047,16 @@
         <v>#N/A</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P20" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="W20" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="b">
         <v>0</v>
       </c>
@@ -2999,10 +3065,10 @@
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F21" s="5" t="b">
         <v>0</v>
@@ -3032,24 +3098,21 @@
         <v>#N/A</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P21" s="6" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q21" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
       <c r="V21" s="5"/>
-      <c r="W21" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="b">
         <v>0</v>
       </c>
@@ -3058,10 +3121,10 @@
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F22" s="5" t="b">
         <v>0</v>
@@ -3091,24 +3154,21 @@
         <v>#N/A</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P22" s="6" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
       <c r="V22" s="5"/>
-      <c r="W22" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="b">
         <v>0</v>
       </c>
@@ -3117,10 +3177,10 @@
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23" s="5" t="b">
         <v>0</v>
@@ -3150,26 +3210,23 @@
         <v>#N/A</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P23" s="6" t="e">
         <v>#N/A</v>
       </c>
       <c r="Q23" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R23" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S23" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
       <c r="V23" s="5"/>
-      <c r="W23" s="5" t="e">
-        <v>#N/A</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3202,16 +3259,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3222,10 +3279,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3236,10 +3293,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3250,10 +3307,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3264,10 +3321,10 @@
         <v>0</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3278,10 +3335,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3292,10 +3349,10 @@
         <v>0</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3306,10 +3363,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3320,10 +3377,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3334,10 +3391,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3348,10 +3405,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3362,7 +3419,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="17">
         <v>1</v>
@@ -3376,7 +3433,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="17">
         <v>0.05</v>
@@ -3390,7 +3447,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="3">
         <v>2</v>
@@ -3404,7 +3461,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="17">
         <v>0.05</v>
@@ -3418,7 +3475,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="17">
         <v>200000</v>
@@ -3432,7 +3489,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="17">
         <v>200</v>
@@ -3446,7 +3503,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="15">
         <v>700</v>
@@ -3460,7 +3517,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="17">
         <v>200</v>
@@ -3473,37 +3530,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{644013CB-DC31-A744-837E-B27655C4D55A}">
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22:M24"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="5" width="40.83203125" customWidth="1"/>
-    <col min="14" max="15" width="35.83203125" customWidth="1"/>
+    <col min="16" max="19" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>8</v>
@@ -3512,26 +3569,34 @@
         <v>9</v>
       </c>
       <c r="I1" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="M1" s="1"/>
-      <c r="N1" s="68" t="s">
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q1" s="65" t="s">
         <v>155</v>
       </c>
-      <c r="O1" s="73" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="R1" s="72" t="s">
+        <v>163</v>
+      </c>
+      <c r="S1" s="72" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="b">
         <v>1</v>
       </c>
@@ -3539,13 +3604,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>23</v>
-      </c>
       <c r="E2" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -3553,14 +3618,20 @@
       <c r="I2" s="3">
         <v>1</v>
       </c>
-      <c r="N2" s="69" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="74" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="88" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="88" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="b">
         <v>1</v>
       </c>
@@ -3568,13 +3639,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -3582,14 +3653,20 @@
       <c r="I3" s="3">
         <v>1</v>
       </c>
-      <c r="N3" s="69" t="s">
-        <v>119</v>
-      </c>
-      <c r="O3" s="74" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q3" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="R3" s="88" t="s">
+        <v>118</v>
+      </c>
+      <c r="S3" s="88" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="b">
         <v>1</v>
       </c>
@@ -3597,13 +3674,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -3611,14 +3688,20 @@
       <c r="I4" s="3">
         <v>1</v>
       </c>
-      <c r="N4" s="69" t="s">
-        <v>15</v>
-      </c>
-      <c r="O4" s="74" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4" s="66" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="66" t="s">
+        <v>14</v>
+      </c>
+      <c r="R4" s="88" t="s">
+        <v>14</v>
+      </c>
+      <c r="S4" s="88" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="b">
         <v>1</v>
       </c>
@@ -3626,13 +3709,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -3640,14 +3723,20 @@
       <c r="I5" s="3">
         <v>1</v>
       </c>
-      <c r="N5" s="70" t="s">
-        <v>103</v>
-      </c>
-      <c r="O5" s="75" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q5" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="R5" s="89" t="s">
+        <v>102</v>
+      </c>
+      <c r="S5" s="89" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="b">
         <v>1</v>
       </c>
@@ -3655,13 +3744,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -3669,14 +3758,20 @@
       <c r="I6" s="3">
         <v>1</v>
       </c>
-      <c r="N6" s="70" t="s">
-        <v>141</v>
-      </c>
-      <c r="O6" s="75" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P6" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q6" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="R6" s="89" t="s">
+        <v>139</v>
+      </c>
+      <c r="S6" s="89" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="b">
         <v>1</v>
       </c>
@@ -3684,13 +3779,13 @@
         <v>0</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -3698,14 +3793,20 @@
       <c r="I7" s="3">
         <v>1</v>
       </c>
-      <c r="N7" s="70" t="s">
-        <v>141</v>
-      </c>
-      <c r="O7" s="75" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P7" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q7" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="R7" s="89" t="s">
+        <v>139</v>
+      </c>
+      <c r="S7" s="89" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="b">
         <v>1</v>
       </c>
@@ -3713,13 +3814,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -3727,14 +3828,20 @@
       <c r="I8" s="3">
         <v>1</v>
       </c>
-      <c r="N8" s="69" t="s">
-        <v>101</v>
-      </c>
-      <c r="O8" s="74" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P8" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q8" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="R8" s="88" t="s">
+        <v>100</v>
+      </c>
+      <c r="S8" s="88" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="b">
         <v>1</v>
       </c>
@@ -3742,13 +3849,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -3756,14 +3863,20 @@
       <c r="I9" s="3">
         <v>1</v>
       </c>
-      <c r="N9" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="O9" s="74" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P9" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q9" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="R9" s="88" t="s">
+        <v>44</v>
+      </c>
+      <c r="S9" s="88" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="b">
         <v>1</v>
       </c>
@@ -3771,13 +3884,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -3785,14 +3898,20 @@
       <c r="I10" s="3">
         <v>1</v>
       </c>
-      <c r="N10" s="70" t="s">
-        <v>141</v>
-      </c>
-      <c r="O10" s="75" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q10" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="R10" s="89" t="s">
+        <v>139</v>
+      </c>
+      <c r="S10" s="89" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="b">
         <v>1</v>
       </c>
@@ -3800,13 +3919,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -3814,14 +3933,20 @@
       <c r="I11" s="3">
         <v>1</v>
       </c>
-      <c r="N11" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="O11" s="74" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P11" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q11" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="R11" s="88" t="s">
+        <v>44</v>
+      </c>
+      <c r="S11" s="88" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="b">
         <v>1</v>
       </c>
@@ -3829,22 +3954,22 @@
         <v>1</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="17">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="17">
-        <v>1</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="I12" s="3">
         <v>10</v>
@@ -3855,20 +3980,32 @@
       <c r="K12" s="1">
         <v>10</v>
       </c>
-      <c r="L12" s="68">
+      <c r="L12" s="65">
         <v>10</v>
       </c>
-      <c r="M12" s="82">
+      <c r="M12" s="65">
         <v>7</v>
       </c>
-      <c r="N12" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="O12" s="76" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N12" s="72">
+        <v>5</v>
+      </c>
+      <c r="O12" s="72">
+        <v>6</v>
+      </c>
+      <c r="P12" s="86" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q12" s="87" t="s">
+        <v>149</v>
+      </c>
+      <c r="R12" s="90" t="s">
+        <v>154</v>
+      </c>
+      <c r="S12" s="90" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="b">
         <v>1</v>
       </c>
@@ -3876,42 +4013,54 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="17">
         <v>0.05</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I13" s="3">
         <v>4</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="80">
+      <c r="L13" s="70">
         <v>2</v>
       </c>
-      <c r="M13" s="83">
+      <c r="M13" s="70">
         <v>4</v>
       </c>
-      <c r="N13" s="64" t="s">
-        <v>138</v>
-      </c>
-      <c r="O13" s="76" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N13" s="73">
+        <v>4</v>
+      </c>
+      <c r="O13" s="73">
+        <v>4</v>
+      </c>
+      <c r="P13" s="86" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q13" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="R13" s="91" t="s">
+        <v>114</v>
+      </c>
+      <c r="S13" s="91" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="b">
         <v>1</v>
       </c>
@@ -3919,22 +4068,22 @@
         <v>1</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="3">
         <v>2</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I14" s="3">
         <v>3</v>
@@ -3945,20 +4094,32 @@
       <c r="K14" s="1">
         <v>3</v>
       </c>
-      <c r="L14" s="80">
+      <c r="L14" s="70">
         <v>3</v>
       </c>
-      <c r="M14" s="83">
+      <c r="M14" s="70">
         <v>3</v>
       </c>
-      <c r="N14" s="64" t="s">
-        <v>35</v>
-      </c>
-      <c r="O14" s="77" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N14" s="73">
+        <v>3</v>
+      </c>
+      <c r="O14" s="73">
+        <v>3</v>
+      </c>
+      <c r="P14" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q14" s="85" t="s">
+        <v>34</v>
+      </c>
+      <c r="R14" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="S14" s="92" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="b">
         <v>1</v>
       </c>
@@ -3966,22 +4127,22 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="17">
         <v>0.05</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="H15" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I15" s="3">
         <v>4</v>
@@ -3992,20 +4153,32 @@
       <c r="K15" s="1">
         <v>4</v>
       </c>
-      <c r="L15" s="81">
+      <c r="L15" s="71">
         <v>4</v>
       </c>
-      <c r="M15" s="84">
+      <c r="M15" s="71">
         <v>4</v>
       </c>
-      <c r="N15" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="O15" s="77" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N15" s="74">
+        <v>4</v>
+      </c>
+      <c r="O15" s="74">
+        <v>4</v>
+      </c>
+      <c r="P15" s="86" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q15" s="85" t="s">
+        <v>114</v>
+      </c>
+      <c r="R15" s="92" t="s">
+        <v>114</v>
+      </c>
+      <c r="S15" s="92" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="b">
         <v>1</v>
       </c>
@@ -4013,7 +4186,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="17">
         <v>200000</v>
@@ -4022,21 +4195,27 @@
         <v>200000</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="3">
         <v>1</v>
       </c>
-      <c r="N16" s="71">
+      <c r="P16" s="68">
         <v>200000</v>
       </c>
-      <c r="O16" s="78">
+      <c r="Q16" s="68">
         <v>200000</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R16" s="93">
+        <v>200000</v>
+      </c>
+      <c r="S16" s="93">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="b">
         <v>1</v>
       </c>
@@ -4044,34 +4223,40 @@
         <v>1</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="17">
         <v>200</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I17" s="3">
         <v>5</v>
       </c>
-      <c r="N17" s="71">
+      <c r="P17" s="68">
         <v>200</v>
       </c>
-      <c r="O17" s="78">
+      <c r="Q17" s="68">
         <v>200</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R17" s="93">
+        <v>200</v>
+      </c>
+      <c r="S17" s="93">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="b">
         <v>1</v>
       </c>
@@ -4079,7 +4264,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="15">
         <v>700</v>
@@ -4093,14 +4278,20 @@
       <c r="I18" s="3">
         <v>1</v>
       </c>
-      <c r="N18" s="69">
+      <c r="P18" s="66">
         <v>700</v>
       </c>
-      <c r="O18" s="74">
+      <c r="Q18" s="66">
         <v>700</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R18" s="88">
+        <v>700</v>
+      </c>
+      <c r="S18" s="88">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="b">
         <v>1</v>
       </c>
@@ -4108,7 +4299,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="17">
         <v>200</v>
@@ -4122,14 +4313,20 @@
       <c r="I19" s="3">
         <v>1</v>
       </c>
-      <c r="N19" s="72">
+      <c r="P19" s="69">
         <v>200</v>
       </c>
-      <c r="O19" s="79">
+      <c r="Q19" s="69">
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R19" s="94">
+        <v>200</v>
+      </c>
+      <c r="S19" s="94">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="9"/>
@@ -4139,16 +4336,16 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="3"/>
-      <c r="N20" s="17"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P20" s="17"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H21" s="37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H22" s="34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I22" s="30">
         <f>PRODUCT(I2:I19)</f>
@@ -4162,19 +4359,26 @@
         <f>PRODUCT(K2:K19)</f>
         <v>120</v>
       </c>
-      <c r="L22" s="65">
+      <c r="L22" s="63">
         <f>PRODUCT(L2:L19)</f>
         <v>240</v>
       </c>
-      <c r="M22" s="85">
+      <c r="M22" s="63">
         <f>PRODUCT(M2:M19)</f>
         <v>336</v>
       </c>
-      <c r="N22" s="63"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N22" s="110">
+        <f>PRODUCT(N2:N19)</f>
+        <v>240</v>
+      </c>
+      <c r="O22" s="75">
+        <f>PRODUCT(O2:O19)</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H23" s="35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I23" s="32">
         <f>3*I22</f>
@@ -4188,202 +4392,328 @@
         <f>3*K22</f>
         <v>360</v>
       </c>
-      <c r="L23" s="66">
+      <c r="L23" s="64">
         <f>3*L22</f>
         <v>720</v>
       </c>
-      <c r="M23" s="86">
+      <c r="M23" s="64">
         <f>3*M22</f>
         <v>1008</v>
       </c>
-      <c r="N23" s="63"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N23" s="111">
+        <f>3*N22</f>
+        <v>720</v>
+      </c>
+      <c r="O23" s="76">
+        <f>3*O22</f>
+        <v>864</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H24" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="I24" s="33">
+        <v>127</v>
+      </c>
+      <c r="I24" s="32">
         <f>5*I22</f>
         <v>12000</v>
       </c>
-      <c r="J24" s="33">
+      <c r="J24" s="32">
         <f>5*J22</f>
         <v>450</v>
       </c>
-      <c r="K24" s="33">
+      <c r="K24" s="32">
         <f>5*K22</f>
         <v>600</v>
       </c>
-      <c r="L24" s="67">
+      <c r="L24" s="96">
         <f>5*L22</f>
         <v>1200</v>
       </c>
-      <c r="M24" s="87">
+      <c r="M24" s="96">
         <f>5*M22</f>
         <v>1680</v>
       </c>
-      <c r="N24" s="63"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="N26" s="37" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="N27" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="O27" s="30" t="s">
+      <c r="N24" s="111">
+        <f>5*N22</f>
+        <v>1200</v>
+      </c>
+      <c r="O24" s="76">
+        <f>5*O22</f>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H25" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="I25" s="107">
+        <f>4*I22</f>
+        <v>9600</v>
+      </c>
+      <c r="J25" s="107">
+        <f>4*J22</f>
+        <v>360</v>
+      </c>
+      <c r="K25" s="107">
+        <f>4*K22</f>
+        <v>480</v>
+      </c>
+      <c r="L25" s="108">
+        <f>4*L22</f>
+        <v>960</v>
+      </c>
+      <c r="M25" s="108">
+        <f>4*M22</f>
+        <v>1344</v>
+      </c>
+      <c r="N25" s="112">
+        <f>4*N22</f>
+        <v>960</v>
+      </c>
+      <c r="O25" s="109">
+        <f>4*O22</f>
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H26" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="I26" s="33">
+        <f>6*I22</f>
+        <v>14400</v>
+      </c>
+      <c r="J26" s="33">
+        <f t="shared" ref="J26:N26" si="0">6*J22</f>
+        <v>540</v>
+      </c>
+      <c r="K26" s="33">
+        <f t="shared" si="0"/>
+        <v>720</v>
+      </c>
+      <c r="L26" s="97">
+        <f t="shared" si="0"/>
+        <v>1440</v>
+      </c>
+      <c r="M26" s="97">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="N26" s="113">
+        <f t="shared" si="0"/>
+        <v>1440</v>
+      </c>
+      <c r="O26" s="77">
+        <f t="shared" ref="O26" si="1">6*O22</f>
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H27" s="84"/>
+      <c r="I27" s="84"/>
+      <c r="J27" s="84"/>
+      <c r="N27" s="84"/>
+      <c r="O27" s="84"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P28" s="37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P29" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q29" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="P27" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q27" s="31" t="s">
+      <c r="R29" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="S29" s="31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P30" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q30" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="R30" s="39">
+        <v>30</v>
+      </c>
+      <c r="S30" s="40" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P31" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q31" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="R31" s="39">
+        <v>20</v>
+      </c>
+      <c r="S31" s="40" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P32" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q32" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="R32" s="39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S32" s="40" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P33" s="35" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="N28" s="35" t="s">
+      <c r="Q33" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="R33" s="44">
+        <v>30</v>
+      </c>
+      <c r="S33" s="99" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P34" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q34" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="R34" s="44">
+        <v>50</v>
+      </c>
+      <c r="S34" s="99" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P35" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q35" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="O28" s="39" t="s">
+      <c r="R35" s="44">
+        <v>20</v>
+      </c>
+      <c r="S35" s="99" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P36" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q36" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="R36" s="44">
+        <v>30</v>
+      </c>
+      <c r="S36" s="99" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P37" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q37" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="P28" s="39">
-        <v>30</v>
-      </c>
-      <c r="Q28" s="40" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="N29" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="O29" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="P29" s="39">
-        <v>20</v>
-      </c>
-      <c r="Q29" s="40" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="N30" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="O30" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="P30" s="39" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q30" s="40" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="N31" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="O31" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="P31" s="44">
-        <v>30</v>
-      </c>
-      <c r="Q31" s="40" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="N32" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="O32" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="P32" s="44">
-        <v>50</v>
-      </c>
-      <c r="Q32" s="40" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="N33" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="O33" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="P33" s="44">
-        <v>20</v>
-      </c>
-      <c r="Q33" s="40" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="N34" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="O34" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="P34" s="44">
-        <v>30</v>
-      </c>
-      <c r="Q34" s="40" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="N35" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="O35" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="P35" s="45" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q35" s="43" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="9"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R37" s="45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S37" s="100" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C38" s="9"/>
+      <c r="P38" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q38" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="R38" s="39">
+        <v>50</v>
+      </c>
+      <c r="S38" s="40" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="9"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C39" s="1"/>
+      <c r="P39" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q39" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="R39" s="39">
+        <v>30</v>
+      </c>
+      <c r="S39" s="40" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C40" s="9"/>
+      <c r="P40" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q40" s="98" t="s">
+        <v>130</v>
+      </c>
+      <c r="R40" s="98" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S40" s="43" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="9"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C41" s="1"/>
+      <c r="P41" s="84"/>
+      <c r="Q41" s="84"/>
+      <c r="R41" s="84"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="9"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4394,242 +4724,330 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E14 N14" twoDigitTextYear="1"/>
+    <ignoredError sqref="E14 P14" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A19AA3B-A7B0-864C-B5E4-F8D7A1F6D4E7}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
-    </sheetView>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="35.83203125" customWidth="1"/>
+    <col min="1" max="7" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="95" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="95" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="49">
+        <v>1</v>
+      </c>
+      <c r="C13" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="59" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="50" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="C4" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="50" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="60" t="s">
-        <v>141</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="60" t="s">
-        <v>141</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="50" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="C11" s="60" t="s">
-        <v>141</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="50" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="49">
-        <v>1</v>
-      </c>
-      <c r="C13" s="60" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="59" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="83" t="s">
+        <v>154</v>
+      </c>
+      <c r="F13" s="83" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="49">
         <v>0.05</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D14" s="59" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="E14" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="59" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="49">
         <v>2</v>
       </c>
       <c r="C15" s="60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="49">
         <v>0.05</v>
       </c>
       <c r="C16" s="60" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="53" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" s="49">
         <v>200000</v>
@@ -4640,10 +5058,16 @@
       <c r="D17" s="54">
         <v>200000</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="54">
+        <v>200000</v>
+      </c>
+      <c r="F17" s="54">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="49">
         <v>200</v>
@@ -4654,10 +5078,16 @@
       <c r="D18" s="54">
         <v>200</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="54">
+        <v>200</v>
+      </c>
+      <c r="F18" s="54">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="49">
         <v>700</v>
@@ -4668,103 +5098,130 @@
       <c r="D19" s="50">
         <v>700</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="50">
+        <v>700</v>
+      </c>
+      <c r="F19" s="50">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="56">
         <v>200</v>
       </c>
-      <c r="C20" s="88">
+      <c r="C20" s="78">
         <v>200</v>
       </c>
       <c r="D20" s="57">
         <v>200</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="57">
+        <v>200</v>
+      </c>
+      <c r="F20" s="57">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="47" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B22" s="47"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" s="38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" s="35" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C24" s="61" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D24" s="44">
         <v>30</v>
       </c>
       <c r="E24" s="40" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+      <c r="F24" s="40" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" s="35" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C25" s="61" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D25" s="44">
         <v>50</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B26" s="35" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C26" s="61" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D26" s="44">
         <v>20</v>
       </c>
       <c r="E26" s="40" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+      <c r="F26" s="40" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" s="35" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C27" s="61" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D27" s="44">
         <v>30</v>
       </c>
       <c r="E27" s="40" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="F27" s="40" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" s="36" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C28" s="62" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D28" s="45" t="e">
         <v>#N/A</v>
@@ -4772,58 +5229,126 @@
       <c r="E28" s="43" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="43" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="47" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B30" s="47"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B31" s="34" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>156</v>
-      </c>
-      <c r="D31" s="89" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+      <c r="D31" s="79" t="s">
+        <v>152</v>
+      </c>
+      <c r="E31" s="79" t="s">
+        <v>161</v>
+      </c>
+      <c r="F31" s="79" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="C32" s="91">
+        <v>119</v>
+      </c>
+      <c r="C32" s="80">
         <v>240</v>
       </c>
-      <c r="D32" s="89">
+      <c r="D32" s="79">
         <v>336</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="92" t="s">
-        <v>158</v>
-      </c>
-      <c r="C33" s="93">
+      <c r="E32" s="79">
+        <v>240</v>
+      </c>
+      <c r="F32" s="79">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="81">
         <f>C32*2</f>
         <v>480</v>
       </c>
-      <c r="D33" s="94">
+      <c r="D33" s="82">
         <f>D32*2</f>
         <v>672</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="82">
+        <f>E32*2</f>
+        <v>480</v>
+      </c>
+      <c r="F33" s="82">
+        <f>F32*2</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="C34" s="6">
+        <v>127</v>
+      </c>
+      <c r="C34" s="101">
         <v>1200</v>
       </c>
-      <c r="D34" s="90">
+      <c r="D34" s="102">
         <v>1680</v>
       </c>
+      <c r="E34" s="103">
+        <v>1200</v>
+      </c>
+      <c r="F34" s="103">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="101">
+        <v>960</v>
+      </c>
+      <c r="D35" s="102">
+        <v>1344</v>
+      </c>
+      <c r="E35" s="103">
+        <v>960</v>
+      </c>
+      <c r="F35" s="103">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="C36" s="104">
+        <v>1440</v>
+      </c>
+      <c r="D36" s="105">
+        <v>2016</v>
+      </c>
+      <c r="E36" s="106">
+        <v>1440</v>
+      </c>
+      <c r="F36" s="106">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="84"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="84"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Continued job-array work: Getting close: Have got the multi-list code working, and the new separate submission and run scripts working; #TBC #TOMORROW
</commit_message>
<xml_diff>
--- a/results/2022-1101/notebook/trinity-parameters.xlsx
+++ b/results/2022-1101/notebook/trinity-parameters.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavatt/projects-etc/2022_transcriptome-construction/results/2022-1101/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC87024-8CDD-F94F-A80C-96CE13FD31EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8485A59C-470C-5341-834C-2B71AA71D066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="3600" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{8F9F2F58-FFA3-AE48-BF61-DF943E6DC9C3}"/>
+    <workbookView xWindow="7600" yWindow="3580" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{8F9F2F58-FFA3-AE48-BF61-DF943E6DC9C3}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
     <sheet name="draft_2022-1201" sheetId="2" r:id="rId2"/>
-    <sheet name="draft_2023-0111_draft" sheetId="3" r:id="rId3"/>
-    <sheet name="draft_2023-0111_succinct" sheetId="4" r:id="rId4"/>
+    <sheet name="draft_2023-0111-012X_draft" sheetId="3" r:id="rId3"/>
+    <sheet name="draft_2023-0111-012X_succinct" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="164">
   <si>
     <t>parameter</t>
   </si>
@@ -1330,7 +1330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1513,11 +1513,10 @@
     <xf numFmtId="0" fontId="19" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1544,7 +1543,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1559,16 +1557,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1581,6 +1573,22 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3532,8 +3540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{644013CB-DC31-A744-837E-B27655C4D55A}">
   <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3624,10 +3632,10 @@
       <c r="Q2" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="88" t="s">
+      <c r="R2" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="88" t="s">
+      <c r="S2" s="87" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3659,10 +3667,10 @@
       <c r="Q3" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="R3" s="88" t="s">
+      <c r="R3" s="87" t="s">
         <v>118</v>
       </c>
-      <c r="S3" s="88" t="s">
+      <c r="S3" s="87" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3694,10 +3702,10 @@
       <c r="Q4" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="88" t="s">
+      <c r="R4" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="S4" s="88" t="s">
+      <c r="S4" s="87" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3729,10 +3737,10 @@
       <c r="Q5" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="R5" s="89" t="s">
+      <c r="R5" s="88" t="s">
         <v>102</v>
       </c>
-      <c r="S5" s="89" t="s">
+      <c r="S5" s="88" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3764,10 +3772,10 @@
       <c r="Q6" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="R6" s="89" t="s">
+      <c r="R6" s="88" t="s">
         <v>139</v>
       </c>
-      <c r="S6" s="89" t="s">
+      <c r="S6" s="88" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3799,10 +3807,10 @@
       <c r="Q7" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="R7" s="89" t="s">
+      <c r="R7" s="88" t="s">
         <v>139</v>
       </c>
-      <c r="S7" s="89" t="s">
+      <c r="S7" s="88" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3834,10 +3842,10 @@
       <c r="Q8" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="R8" s="88" t="s">
+      <c r="R8" s="87" t="s">
         <v>100</v>
       </c>
-      <c r="S8" s="88" t="s">
+      <c r="S8" s="87" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3869,10 +3877,10 @@
       <c r="Q9" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="R9" s="88" t="s">
+      <c r="R9" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="S9" s="88" t="s">
+      <c r="S9" s="87" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3904,10 +3912,10 @@
       <c r="Q10" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="R10" s="89" t="s">
+      <c r="R10" s="88" t="s">
         <v>139</v>
       </c>
-      <c r="S10" s="89" t="s">
+      <c r="S10" s="88" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3939,10 +3947,10 @@
       <c r="Q11" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="R11" s="88" t="s">
+      <c r="R11" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="S11" s="88" t="s">
+      <c r="S11" s="87" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3992,16 +4000,16 @@
       <c r="O12" s="72">
         <v>6</v>
       </c>
-      <c r="P12" s="86" t="s">
+      <c r="P12" s="85" t="s">
         <v>117</v>
       </c>
-      <c r="Q12" s="87" t="s">
+      <c r="Q12" s="86" t="s">
         <v>149</v>
       </c>
-      <c r="R12" s="90" t="s">
+      <c r="R12" s="89" t="s">
         <v>154</v>
       </c>
-      <c r="S12" s="90" t="s">
+      <c r="S12" s="89" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4047,16 +4055,16 @@
       <c r="O13" s="73">
         <v>4</v>
       </c>
-      <c r="P13" s="86" t="s">
+      <c r="P13" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="Q13" s="87" t="s">
+      <c r="Q13" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="R13" s="91" t="s">
+      <c r="R13" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="S13" s="91" t="s">
+      <c r="S13" s="90" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4106,16 +4114,16 @@
       <c r="O14" s="73">
         <v>3</v>
       </c>
-      <c r="P14" s="86" t="s">
+      <c r="P14" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="Q14" s="85" t="s">
+      <c r="Q14" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="R14" s="92" t="s">
+      <c r="R14" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="S14" s="92" t="s">
+      <c r="S14" s="91" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4165,16 +4173,16 @@
       <c r="O15" s="74">
         <v>4</v>
       </c>
-      <c r="P15" s="86" t="s">
+      <c r="P15" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="Q15" s="85" t="s">
+      <c r="Q15" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="R15" s="92" t="s">
+      <c r="R15" s="91" t="s">
         <v>114</v>
       </c>
-      <c r="S15" s="92" t="s">
+      <c r="S15" s="91" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4208,10 +4216,10 @@
       <c r="Q16" s="68">
         <v>200000</v>
       </c>
-      <c r="R16" s="93">
+      <c r="R16" s="92">
         <v>200000</v>
       </c>
-      <c r="S16" s="93">
+      <c r="S16" s="92">
         <v>200000</v>
       </c>
     </row>
@@ -4249,10 +4257,10 @@
       <c r="Q17" s="68">
         <v>200</v>
       </c>
-      <c r="R17" s="93">
+      <c r="R17" s="92">
         <v>200</v>
       </c>
-      <c r="S17" s="93">
+      <c r="S17" s="92">
         <v>200</v>
       </c>
     </row>
@@ -4284,10 +4292,10 @@
       <c r="Q18" s="66">
         <v>700</v>
       </c>
-      <c r="R18" s="88">
+      <c r="R18" s="87">
         <v>700</v>
       </c>
-      <c r="S18" s="88">
+      <c r="S18" s="87">
         <v>700</v>
       </c>
     </row>
@@ -4319,10 +4327,10 @@
       <c r="Q19" s="69">
         <v>200</v>
       </c>
-      <c r="R19" s="94">
+      <c r="R19" s="93">
         <v>200</v>
       </c>
-      <c r="S19" s="94">
+      <c r="S19" s="93">
         <v>200</v>
       </c>
     </row>
@@ -4348,31 +4356,31 @@
         <v>119</v>
       </c>
       <c r="I22" s="30">
-        <f>PRODUCT(I2:I19)</f>
+        <f t="shared" ref="I22:O22" si="0">PRODUCT(I2:I19)</f>
         <v>2400</v>
       </c>
       <c r="J22" s="30">
-        <f>PRODUCT(J2:J19)</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="K22" s="30">
-        <f>PRODUCT(K2:K19)</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="L22" s="63">
-        <f>PRODUCT(L2:L19)</f>
+        <f t="shared" si="0"/>
         <v>240</v>
       </c>
       <c r="M22" s="63">
-        <f>PRODUCT(M2:M19)</f>
+        <f t="shared" si="0"/>
         <v>336</v>
       </c>
-      <c r="N22" s="110">
-        <f>PRODUCT(N2:N19)</f>
+      <c r="N22" s="106">
+        <f t="shared" si="0"/>
         <v>240</v>
       </c>
       <c r="O22" s="75">
-        <f>PRODUCT(O2:O19)</f>
+        <f t="shared" si="0"/>
         <v>288</v>
       </c>
     </row>
@@ -4381,27 +4389,27 @@
         <v>126</v>
       </c>
       <c r="I23" s="32">
-        <f>3*I22</f>
+        <f t="shared" ref="I23:O23" si="1">3*I22</f>
         <v>7200</v>
       </c>
       <c r="J23" s="32">
-        <f>3*J22</f>
+        <f t="shared" si="1"/>
         <v>270</v>
       </c>
       <c r="K23" s="32">
-        <f>3*K22</f>
+        <f t="shared" si="1"/>
         <v>360</v>
       </c>
       <c r="L23" s="64">
-        <f>3*L22</f>
+        <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="M23" s="64">
-        <f>3*M22</f>
+        <f t="shared" si="1"/>
         <v>1008</v>
       </c>
-      <c r="N23" s="111">
-        <f>3*N22</f>
+      <c r="N23" s="107">
+        <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="O23" s="76">
@@ -4414,31 +4422,31 @@
         <v>127</v>
       </c>
       <c r="I24" s="32">
-        <f>5*I22</f>
+        <f t="shared" ref="I24:O24" si="2">5*I22</f>
         <v>12000</v>
       </c>
       <c r="J24" s="32">
-        <f>5*J22</f>
+        <f t="shared" si="2"/>
         <v>450</v>
       </c>
       <c r="K24" s="32">
-        <f>5*K22</f>
+        <f t="shared" si="2"/>
         <v>600</v>
       </c>
-      <c r="L24" s="96">
-        <f>5*L22</f>
+      <c r="L24" s="94">
+        <f t="shared" si="2"/>
         <v>1200</v>
       </c>
-      <c r="M24" s="96">
-        <f>5*M22</f>
+      <c r="M24" s="94">
+        <f t="shared" si="2"/>
         <v>1680</v>
       </c>
-      <c r="N24" s="111">
-        <f>5*N22</f>
+      <c r="N24" s="107">
+        <f t="shared" si="2"/>
         <v>1200</v>
       </c>
       <c r="O24" s="76">
-        <f>5*O22</f>
+        <f t="shared" si="2"/>
         <v>1440</v>
       </c>
     </row>
@@ -4446,32 +4454,32 @@
       <c r="H25" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="I25" s="107">
-        <f>4*I22</f>
+      <c r="I25" s="103">
+        <f t="shared" ref="I25:O25" si="3">4*I22</f>
         <v>9600</v>
       </c>
-      <c r="J25" s="107">
-        <f>4*J22</f>
+      <c r="J25" s="103">
+        <f t="shared" si="3"/>
         <v>360</v>
       </c>
-      <c r="K25" s="107">
-        <f>4*K22</f>
+      <c r="K25" s="103">
+        <f t="shared" si="3"/>
         <v>480</v>
       </c>
-      <c r="L25" s="108">
-        <f>4*L22</f>
+      <c r="L25" s="104">
+        <f t="shared" si="3"/>
         <v>960</v>
       </c>
-      <c r="M25" s="108">
-        <f>4*M22</f>
+      <c r="M25" s="104">
+        <f t="shared" si="3"/>
         <v>1344</v>
       </c>
-      <c r="N25" s="112">
-        <f>4*N22</f>
+      <c r="N25" s="108">
+        <f t="shared" si="3"/>
         <v>960</v>
       </c>
-      <c r="O25" s="109">
-        <f>4*O22</f>
+      <c r="O25" s="105">
+        <f t="shared" si="3"/>
         <v>1152</v>
       </c>
     </row>
@@ -4484,36 +4492,29 @@
         <v>14400</v>
       </c>
       <c r="J26" s="33">
-        <f t="shared" ref="J26:N26" si="0">6*J22</f>
+        <f t="shared" ref="J26:N26" si="4">6*J22</f>
         <v>540</v>
       </c>
       <c r="K26" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>720</v>
       </c>
-      <c r="L26" s="97">
-        <f t="shared" si="0"/>
+      <c r="L26" s="95">
+        <f t="shared" si="4"/>
         <v>1440</v>
       </c>
-      <c r="M26" s="97">
-        <f t="shared" si="0"/>
+      <c r="M26" s="95">
+        <f t="shared" si="4"/>
         <v>2016</v>
       </c>
-      <c r="N26" s="113">
-        <f t="shared" si="0"/>
+      <c r="N26" s="109">
+        <f t="shared" si="4"/>
         <v>1440</v>
       </c>
       <c r="O26" s="77">
-        <f t="shared" ref="O26" si="1">6*O22</f>
+        <f t="shared" ref="O26" si="5">6*O22</f>
         <v>1728</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="H27" s="84"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="84"/>
-      <c r="N27" s="84"/>
-      <c r="O27" s="84"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P28" s="37" t="s">
@@ -4586,7 +4587,7 @@
       <c r="R33" s="44">
         <v>30</v>
       </c>
-      <c r="S33" s="99" t="s">
+      <c r="S33" s="97" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4600,7 +4601,7 @@
       <c r="R34" s="44">
         <v>50</v>
       </c>
-      <c r="S34" s="99" t="s">
+      <c r="S34" s="97" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4614,7 +4615,7 @@
       <c r="R35" s="44">
         <v>20</v>
       </c>
-      <c r="S35" s="99" t="s">
+      <c r="S35" s="97" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4628,7 +4629,7 @@
       <c r="R36" s="44">
         <v>30</v>
       </c>
-      <c r="S36" s="99" t="s">
+      <c r="S36" s="97" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4642,7 +4643,7 @@
       <c r="R37" s="45" t="e">
         <v>#N/A</v>
       </c>
-      <c r="S37" s="100" t="e">
+      <c r="S37" s="98" t="e">
         <v>#N/A</v>
       </c>
     </row>
@@ -4687,10 +4688,10 @@
       <c r="P40" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="Q40" s="98" t="s">
+      <c r="Q40" s="96" t="s">
         <v>130</v>
       </c>
-      <c r="R40" s="98" t="e">
+      <c r="R40" s="96" t="e">
         <v>#N/A</v>
       </c>
       <c r="S40" s="43" t="e">
@@ -4701,9 +4702,6 @@
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="P41" s="84"/>
-      <c r="Q41" s="84"/>
-      <c r="R41" s="84"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
@@ -4731,9 +4729,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A19AA3B-A7B0-864C-B5E4-F8D7A1F6D4E7}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4758,10 +4758,10 @@
       <c r="D2" s="58" t="s">
         <v>148</v>
       </c>
-      <c r="E2" s="95" t="s">
+      <c r="E2" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="F2" s="95" t="s">
+      <c r="F2" s="31" t="s">
         <v>153</v>
       </c>
     </row>
@@ -5144,9 +5144,7 @@
       <c r="E23" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="F23" s="31" t="s">
-        <v>131</v>
-      </c>
+      <c r="F23" s="114"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" s="35" t="s">
@@ -5161,9 +5159,7 @@
       <c r="E24" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="F24" s="40" t="s">
-        <v>132</v>
-      </c>
+      <c r="F24" s="115"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" s="35" t="s">
@@ -5178,9 +5174,7 @@
       <c r="E25" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="F25" s="40" t="s">
-        <v>134</v>
-      </c>
+      <c r="F25" s="115"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B26" s="35" t="s">
@@ -5195,9 +5189,7 @@
       <c r="E26" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="40" t="s">
-        <v>132</v>
-      </c>
+      <c r="F26" s="115"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" s="35" t="s">
@@ -5212,9 +5204,7 @@
       <c r="E27" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="F27" s="40" t="s">
-        <v>134</v>
-      </c>
+      <c r="F27" s="115"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" s="36" t="s">
@@ -5229,9 +5219,7 @@
       <c r="E28" s="43" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F28" s="43" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="F28" s="115"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="47" t="s">
@@ -5263,14 +5251,14 @@
       <c r="C32" s="80">
         <v>240</v>
       </c>
-      <c r="D32" s="79">
+      <c r="D32" s="110">
         <v>336</v>
       </c>
-      <c r="E32" s="79">
+      <c r="E32" s="110">
         <v>240</v>
       </c>
       <c r="F32" s="79">
-        <v>240</v>
+        <v>288</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
@@ -5278,77 +5266,84 @@
         <v>126</v>
       </c>
       <c r="C33" s="81">
-        <f>C32*2</f>
-        <v>480</v>
-      </c>
-      <c r="D33" s="82">
-        <f>D32*2</f>
-        <v>672</v>
-      </c>
-      <c r="E33" s="82">
-        <f>E32*2</f>
-        <v>480</v>
+        <f>C32*3</f>
+        <v>720</v>
+      </c>
+      <c r="D33" s="111">
+        <f>D32*3</f>
+        <v>1008</v>
+      </c>
+      <c r="E33" s="111">
+        <f>E32*3</f>
+        <v>720</v>
       </c>
       <c r="F33" s="82">
-        <f>F32*2</f>
-        <v>480</v>
+        <f>F32*3</f>
+        <v>864</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="C34" s="101">
+      <c r="C34" s="99">
+        <f>C32*5</f>
         <v>1200</v>
       </c>
-      <c r="D34" s="102">
+      <c r="D34" s="99">
+        <f>D32*5</f>
         <v>1680</v>
       </c>
-      <c r="E34" s="103">
+      <c r="E34" s="112">
+        <f>E32*5</f>
         <v>1200</v>
       </c>
-      <c r="F34" s="103">
-        <v>1200</v>
+      <c r="F34" s="100">
+        <f>F32*5</f>
+        <v>1440</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="C35" s="101">
+      <c r="C35" s="99">
+        <f>C32*4</f>
         <v>960</v>
       </c>
-      <c r="D35" s="102">
+      <c r="D35" s="99">
+        <f>D32*4</f>
         <v>1344</v>
       </c>
-      <c r="E35" s="103">
+      <c r="E35" s="112">
+        <f>E32*4</f>
         <v>960</v>
       </c>
-      <c r="F35" s="103">
-        <v>960</v>
+      <c r="F35" s="100">
+        <f>F32*4</f>
+        <v>1152</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="C36" s="104">
+      <c r="C36" s="101">
+        <f>C32*6</f>
         <v>1440</v>
       </c>
-      <c r="D36" s="105">
+      <c r="D36" s="101">
+        <f>D32*6</f>
         <v>2016</v>
       </c>
-      <c r="E36" s="106">
+      <c r="E36" s="113">
+        <f>E32*6</f>
         <v>1440</v>
       </c>
-      <c r="F36" s="106">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C37" s="84"/>
-      <c r="D37" s="84"/>
-      <c r="E37" s="84"/>
+      <c r="F36" s="102">
+        <f>F32*6</f>
+        <v>1728</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Work for 2023-0221: Morning was spent obtaining and analyzing results from rnaQUAST while also check on/starting new jobs and studying in depth the metrics output by rnaQUAST; late morning through the rest of the day (save for a break from 1450 to 1550 for RD's birthday) was spent studying the rnaQUAST results and putting together the presentation for #TOMORROW's lab meeting
</commit_message>
<xml_diff>
--- a/results/2022-1101/notebook/trinity-parameters.xlsx
+++ b/results/2022-1101/notebook/trinity-parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavatt/projects-etc/2022_transcriptome-construction/results/2022-1101/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8485A59C-470C-5341-834C-2B71AA71D066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332B6D3A-88FE-2D44-8409-25FE8E81F1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="3580" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{8F9F2F58-FFA3-AE48-BF61-DF943E6DC9C3}"/>
+    <workbookView xWindow="51220" yWindow="7700" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{8F9F2F58-FFA3-AE48-BF61-DF943E6DC9C3}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="167">
   <si>
     <t>parameter</t>
   </si>
@@ -824,6 +824,15 @@
   </si>
   <si>
     <t>update_2023-0125 (A; final decision)</t>
+  </si>
+  <si>
+    <t>min fraction of average kmer coverage between two iworm contigs required for gluing</t>
+  </si>
+  <si>
+    <t>min number of reads needed to glue two inchworm contigs together</t>
+  </si>
+  <si>
+    <t>fraction of max (iworm pair coverage) for read glue support</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1583,10 +1592,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1915,7 +1920,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <pane xSplit="4" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
@@ -2571,6 +2576,9 @@
       <c r="R11" s="2" t="s">
         <v>112</v>
       </c>
+      <c r="S11" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="b">
@@ -2626,6 +2634,9 @@
       </c>
       <c r="R12" s="2" t="s">
         <v>112</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
@@ -3538,20 +3549,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{644013CB-DC31-A744-837E-B27655C4D55A}">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
-    </sheetView>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="5" width="40.83203125" customWidth="1"/>
-    <col min="16" max="19" width="35.83203125" customWidth="1"/>
+    <col min="17" max="20" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>121</v>
       </c>
@@ -3576,35 +3585,38 @@
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
-      <c r="P1" s="65" t="s">
+      <c r="P1" s="1"/>
+      <c r="Q1" s="65" t="s">
         <v>150</v>
       </c>
-      <c r="Q1" s="65" t="s">
+      <c r="R1" s="65" t="s">
         <v>155</v>
-      </c>
-      <c r="R1" s="72" t="s">
-        <v>163</v>
       </c>
       <c r="S1" s="72" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T1" s="72" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="b">
         <v>1</v>
       </c>
@@ -3623,23 +3635,24 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="3">
-        <v>1</v>
-      </c>
-      <c r="P2" s="66" t="s">
-        <v>22</v>
+      <c r="I2" s="1"/>
+      <c r="J2" s="3">
+        <v>1</v>
       </c>
       <c r="Q2" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="87" t="s">
+      <c r="R2" s="66" t="s">
         <v>22</v>
       </c>
       <c r="S2" s="87" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T2" s="87" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="b">
         <v>1</v>
       </c>
@@ -3658,23 +3671,24 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="3">
-        <v>1</v>
-      </c>
-      <c r="P3" s="66" t="s">
-        <v>118</v>
+      <c r="I3" s="1"/>
+      <c r="J3" s="3">
+        <v>1</v>
       </c>
       <c r="Q3" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="R3" s="87" t="s">
+      <c r="R3" s="66" t="s">
         <v>118</v>
       </c>
       <c r="S3" s="87" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T3" s="87" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="b">
         <v>1</v>
       </c>
@@ -3693,23 +3707,24 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="3">
-        <v>1</v>
-      </c>
-      <c r="P4" s="66" t="s">
-        <v>14</v>
+      <c r="I4" s="1"/>
+      <c r="J4" s="3">
+        <v>1</v>
       </c>
       <c r="Q4" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="87" t="s">
+      <c r="R4" s="66" t="s">
         <v>14</v>
       </c>
       <c r="S4" s="87" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T4" s="87" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="b">
         <v>1</v>
       </c>
@@ -3728,23 +3743,24 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="3">
-        <v>1</v>
-      </c>
-      <c r="P5" s="67" t="s">
-        <v>102</v>
+      <c r="I5" s="1"/>
+      <c r="J5" s="3">
+        <v>1</v>
       </c>
       <c r="Q5" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="R5" s="88" t="s">
+      <c r="R5" s="67" t="s">
         <v>102</v>
       </c>
       <c r="S5" s="88" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T5" s="88" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="b">
         <v>1</v>
       </c>
@@ -3763,23 +3779,24 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="3">
-        <v>1</v>
-      </c>
-      <c r="P6" s="67" t="s">
-        <v>139</v>
+      <c r="I6" s="1"/>
+      <c r="J6" s="3">
+        <v>1</v>
       </c>
       <c r="Q6" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="R6" s="88" t="s">
+      <c r="R6" s="67" t="s">
         <v>139</v>
       </c>
       <c r="S6" s="88" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T6" s="88" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="b">
         <v>1</v>
       </c>
@@ -3798,23 +3815,24 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="3">
-        <v>1</v>
-      </c>
-      <c r="P7" s="67" t="s">
-        <v>139</v>
+      <c r="I7" s="1"/>
+      <c r="J7" s="3">
+        <v>1</v>
       </c>
       <c r="Q7" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="R7" s="88" t="s">
+      <c r="R7" s="67" t="s">
         <v>139</v>
       </c>
       <c r="S7" s="88" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T7" s="88" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="b">
         <v>1</v>
       </c>
@@ -3833,23 +3851,24 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="3">
-        <v>1</v>
-      </c>
-      <c r="P8" s="66" t="s">
-        <v>100</v>
+      <c r="I8" s="1"/>
+      <c r="J8" s="3">
+        <v>1</v>
       </c>
       <c r="Q8" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="R8" s="87" t="s">
+      <c r="R8" s="66" t="s">
         <v>100</v>
       </c>
       <c r="S8" s="87" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T8" s="87" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="b">
         <v>1</v>
       </c>
@@ -3868,23 +3887,24 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="3">
-        <v>1</v>
-      </c>
-      <c r="P9" s="66" t="s">
-        <v>44</v>
+      <c r="I9" s="1"/>
+      <c r="J9" s="3">
+        <v>1</v>
       </c>
       <c r="Q9" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="R9" s="87" t="s">
+      <c r="R9" s="66" t="s">
         <v>44</v>
       </c>
       <c r="S9" s="87" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T9" s="87" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="b">
         <v>1</v>
       </c>
@@ -3903,23 +3923,24 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="3">
-        <v>1</v>
-      </c>
-      <c r="P10" s="67" t="s">
-        <v>139</v>
+      <c r="I10" s="1"/>
+      <c r="J10" s="3">
+        <v>1</v>
       </c>
       <c r="Q10" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="R10" s="88" t="s">
+      <c r="R10" s="67" t="s">
         <v>139</v>
       </c>
       <c r="S10" s="88" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T10" s="88" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="b">
         <v>1</v>
       </c>
@@ -3938,23 +3959,24 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="3">
-        <v>1</v>
-      </c>
-      <c r="P11" s="66" t="s">
-        <v>44</v>
+      <c r="I11" s="1"/>
+      <c r="J11" s="3">
+        <v>1</v>
       </c>
       <c r="Q11" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="R11" s="87" t="s">
+      <c r="R11" s="66" t="s">
         <v>44</v>
       </c>
       <c r="S11" s="87" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T11" s="87" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="b">
         <v>1</v>
       </c>
@@ -3979,41 +4001,42 @@
       <c r="H12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="3">
-        <v>10</v>
-      </c>
-      <c r="J12" s="1">
+      <c r="I12" s="1"/>
+      <c r="J12" s="3">
         <v>10</v>
       </c>
       <c r="K12" s="1">
         <v>10</v>
       </c>
-      <c r="L12" s="65">
+      <c r="L12" s="1">
         <v>10</v>
       </c>
       <c r="M12" s="65">
+        <v>10</v>
+      </c>
+      <c r="N12" s="65">
         <v>7</v>
       </c>
-      <c r="N12" s="72">
+      <c r="O12" s="72">
         <v>5</v>
       </c>
-      <c r="O12" s="72">
+      <c r="P12" s="72">
         <v>6</v>
       </c>
-      <c r="P12" s="85" t="s">
+      <c r="Q12" s="85" t="s">
         <v>117</v>
       </c>
-      <c r="Q12" s="86" t="s">
+      <c r="R12" s="86" t="s">
         <v>149</v>
       </c>
-      <c r="R12" s="89" t="s">
+      <c r="S12" s="89" t="s">
         <v>154</v>
       </c>
-      <c r="S12" s="89" t="s">
+      <c r="T12" s="89" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="b">
         <v>1</v>
       </c>
@@ -4038,37 +4061,40 @@
       <c r="H13" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J13" s="3">
         <v>4</v>
       </c>
-      <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="70">
+      <c r="L13" s="1"/>
+      <c r="M13" s="70">
         <v>2</v>
       </c>
-      <c r="M13" s="70">
-        <v>4</v>
-      </c>
-      <c r="N13" s="73">
+      <c r="N13" s="70">
         <v>4</v>
       </c>
       <c r="O13" s="73">
         <v>4</v>
       </c>
-      <c r="P13" s="85" t="s">
+      <c r="P13" s="73">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="Q13" s="86" t="s">
-        <v>114</v>
-      </c>
-      <c r="R13" s="90" t="s">
+      <c r="R13" s="86" t="s">
         <v>114</v>
       </c>
       <c r="S13" s="90" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T13" s="90" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="b">
         <v>1</v>
       </c>
@@ -4093,41 +4119,44 @@
       <c r="H14" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="I14" s="3">
-        <v>3</v>
-      </c>
-      <c r="J14" s="1">
+      <c r="I14" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="J14" s="3">
         <v>3</v>
       </c>
       <c r="K14" s="1">
         <v>3</v>
       </c>
-      <c r="L14" s="70">
+      <c r="L14" s="1">
         <v>3</v>
       </c>
       <c r="M14" s="70">
         <v>3</v>
       </c>
-      <c r="N14" s="73">
+      <c r="N14" s="70">
         <v>3</v>
       </c>
       <c r="O14" s="73">
         <v>3</v>
       </c>
-      <c r="P14" s="85" t="s">
+      <c r="P14" s="73">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="Q14" s="84" t="s">
-        <v>34</v>
-      </c>
-      <c r="R14" s="91" t="s">
+      <c r="R14" s="84" t="s">
         <v>34</v>
       </c>
       <c r="S14" s="91" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T14" s="91" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="b">
         <v>1</v>
       </c>
@@ -4152,41 +4181,44 @@
       <c r="H15" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J15" s="3">
         <v>4</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <v>3</v>
       </c>
-      <c r="K15" s="1">
-        <v>4</v>
-      </c>
-      <c r="L15" s="71">
+      <c r="L15" s="1">
         <v>4</v>
       </c>
       <c r="M15" s="71">
         <v>4</v>
       </c>
-      <c r="N15" s="74">
+      <c r="N15" s="71">
         <v>4</v>
       </c>
       <c r="O15" s="74">
         <v>4</v>
       </c>
-      <c r="P15" s="85" t="s">
+      <c r="P15" s="74">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="Q15" s="84" t="s">
-        <v>114</v>
-      </c>
-      <c r="R15" s="91" t="s">
+      <c r="R15" s="84" t="s">
         <v>114</v>
       </c>
       <c r="S15" s="91" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T15" s="91" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="b">
         <v>1</v>
       </c>
@@ -4207,23 +4239,24 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="3">
-        <v>1</v>
-      </c>
-      <c r="P16" s="68">
-        <v>200000</v>
+      <c r="I16" s="1"/>
+      <c r="J16" s="3">
+        <v>1</v>
       </c>
       <c r="Q16" s="68">
         <v>200000</v>
       </c>
-      <c r="R16" s="92">
+      <c r="R16" s="68">
         <v>200000</v>
       </c>
       <c r="S16" s="92">
         <v>200000</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T16" s="92">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="b">
         <v>1</v>
       </c>
@@ -4248,23 +4281,24 @@
       <c r="H17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="2"/>
+      <c r="J17" s="3">
         <v>5</v>
-      </c>
-      <c r="P17" s="68">
-        <v>200</v>
       </c>
       <c r="Q17" s="68">
         <v>200</v>
       </c>
-      <c r="R17" s="92">
+      <c r="R17" s="68">
         <v>200</v>
       </c>
       <c r="S17" s="92">
         <v>200</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T17" s="92">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="b">
         <v>1</v>
       </c>
@@ -4283,23 +4317,24 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="3">
-        <v>1</v>
-      </c>
-      <c r="P18" s="66">
-        <v>700</v>
+      <c r="I18" s="1"/>
+      <c r="J18" s="3">
+        <v>1</v>
       </c>
       <c r="Q18" s="66">
         <v>700</v>
       </c>
-      <c r="R18" s="87">
+      <c r="R18" s="66">
         <v>700</v>
       </c>
       <c r="S18" s="87">
         <v>700</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T18" s="87">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="b">
         <v>1</v>
       </c>
@@ -4318,23 +4353,24 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="3">
-        <v>1</v>
-      </c>
-      <c r="P19" s="69">
-        <v>200</v>
+      <c r="I19" s="1"/>
+      <c r="J19" s="3">
+        <v>1</v>
       </c>
       <c r="Q19" s="69">
         <v>200</v>
       </c>
-      <c r="R19" s="93">
+      <c r="R19" s="69">
         <v>200</v>
       </c>
       <c r="S19" s="93">
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T19" s="93">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="9"/>
@@ -4343,372 +4379,379 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="3"/>
-      <c r="P20" s="17"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I20" s="1"/>
+      <c r="J20" s="3"/>
+      <c r="Q20" s="17"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H21" s="37" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I21" s="37"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H22" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="I22" s="30">
-        <f t="shared" ref="I22:O22" si="0">PRODUCT(I2:I19)</f>
+      <c r="I22" s="34"/>
+      <c r="J22" s="30">
+        <f t="shared" ref="J22:P22" si="0">PRODUCT(J2:J19)</f>
         <v>2400</v>
       </c>
-      <c r="J22" s="30">
+      <c r="K22" s="30">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="K22" s="30">
+      <c r="L22" s="30">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="L22" s="63">
+      <c r="M22" s="63">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
-      <c r="M22" s="63">
+      <c r="N22" s="63">
         <f t="shared" si="0"/>
         <v>336</v>
       </c>
-      <c r="N22" s="106">
+      <c r="O22" s="106">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
-      <c r="O22" s="75">
+      <c r="P22" s="75">
         <f t="shared" si="0"/>
         <v>288</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H23" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="I23" s="32">
-        <f t="shared" ref="I23:O23" si="1">3*I22</f>
+      <c r="I23" s="35"/>
+      <c r="J23" s="32">
+        <f t="shared" ref="J23:O23" si="1">3*J22</f>
         <v>7200</v>
       </c>
-      <c r="J23" s="32">
+      <c r="K23" s="32">
         <f t="shared" si="1"/>
         <v>270</v>
       </c>
-      <c r="K23" s="32">
+      <c r="L23" s="32">
         <f t="shared" si="1"/>
         <v>360</v>
       </c>
-      <c r="L23" s="64">
+      <c r="M23" s="64">
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
-      <c r="M23" s="64">
+      <c r="N23" s="64">
         <f t="shared" si="1"/>
         <v>1008</v>
       </c>
-      <c r="N23" s="107">
+      <c r="O23" s="107">
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
-      <c r="O23" s="76">
-        <f>3*O22</f>
+      <c r="P23" s="76">
+        <f>3*P22</f>
         <v>864</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H24" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="I24" s="32">
-        <f t="shared" ref="I24:O24" si="2">5*I22</f>
+      <c r="I24" s="36"/>
+      <c r="J24" s="32">
+        <f t="shared" ref="J24:P24" si="2">5*J22</f>
         <v>12000</v>
       </c>
-      <c r="J24" s="32">
+      <c r="K24" s="32">
         <f t="shared" si="2"/>
         <v>450</v>
       </c>
-      <c r="K24" s="32">
+      <c r="L24" s="32">
         <f t="shared" si="2"/>
         <v>600</v>
       </c>
-      <c r="L24" s="94">
+      <c r="M24" s="94">
         <f t="shared" si="2"/>
         <v>1200</v>
       </c>
-      <c r="M24" s="94">
+      <c r="N24" s="94">
         <f t="shared" si="2"/>
         <v>1680</v>
       </c>
-      <c r="N24" s="107">
+      <c r="O24" s="107">
         <f t="shared" si="2"/>
         <v>1200</v>
       </c>
-      <c r="O24" s="76">
+      <c r="P24" s="76">
         <f t="shared" si="2"/>
         <v>1440</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H25" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="I25" s="103">
-        <f t="shared" ref="I25:O25" si="3">4*I22</f>
+      <c r="I25" s="36"/>
+      <c r="J25" s="103">
+        <f t="shared" ref="J25:P25" si="3">4*J22</f>
         <v>9600</v>
       </c>
-      <c r="J25" s="103">
+      <c r="K25" s="103">
         <f t="shared" si="3"/>
         <v>360</v>
       </c>
-      <c r="K25" s="103">
+      <c r="L25" s="103">
         <f t="shared" si="3"/>
         <v>480</v>
       </c>
-      <c r="L25" s="104">
+      <c r="M25" s="104">
         <f t="shared" si="3"/>
         <v>960</v>
       </c>
-      <c r="M25" s="104">
+      <c r="N25" s="104">
         <f t="shared" si="3"/>
         <v>1344</v>
       </c>
-      <c r="N25" s="108">
+      <c r="O25" s="108">
         <f t="shared" si="3"/>
         <v>960</v>
       </c>
-      <c r="O25" s="105">
+      <c r="P25" s="105">
         <f t="shared" si="3"/>
         <v>1152</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H26" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="I26" s="33">
-        <f>6*I22</f>
+      <c r="I26" s="36"/>
+      <c r="J26" s="33">
+        <f>6*J22</f>
         <v>14400</v>
       </c>
-      <c r="J26" s="33">
-        <f t="shared" ref="J26:N26" si="4">6*J22</f>
+      <c r="K26" s="33">
+        <f t="shared" ref="K26:O26" si="4">6*K22</f>
         <v>540</v>
       </c>
-      <c r="K26" s="33">
+      <c r="L26" s="33">
         <f t="shared" si="4"/>
         <v>720</v>
       </c>
-      <c r="L26" s="95">
+      <c r="M26" s="95">
         <f t="shared" si="4"/>
         <v>1440</v>
       </c>
-      <c r="M26" s="95">
+      <c r="N26" s="95">
         <f t="shared" si="4"/>
         <v>2016</v>
       </c>
-      <c r="N26" s="109">
+      <c r="O26" s="109">
         <f t="shared" si="4"/>
         <v>1440</v>
       </c>
-      <c r="O26" s="77">
-        <f t="shared" ref="O26" si="5">6*O22</f>
+      <c r="P26" s="77">
+        <f t="shared" ref="P26" si="5">6*P22</f>
         <v>1728</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P28" s="37" t="s">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q28" s="37" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P29" s="38" t="s">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q29" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="Q29" s="30" t="s">
+      <c r="R29" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="R29" s="30" t="s">
+      <c r="S29" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="S29" s="31" t="s">
+      <c r="T29" s="31" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P30" s="35" t="s">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q30" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="Q30" s="39" t="s">
+      <c r="R30" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="R30" s="39">
+      <c r="S30" s="39">
         <v>30</v>
       </c>
-      <c r="S30" s="40" t="s">
+      <c r="T30" s="40" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P31" s="35" t="s">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q31" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="Q31" s="39" t="s">
+      <c r="R31" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="R31" s="39">
+      <c r="S31" s="39">
         <v>20</v>
       </c>
-      <c r="S31" s="40" t="s">
+      <c r="T31" s="40" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P32" s="35" t="s">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q32" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="Q32" s="39" t="s">
+      <c r="R32" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="R32" s="39" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="S32" s="40" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P33" s="35" t="s">
+      <c r="S32" s="39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T32" s="40" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q33" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="Q33" s="41" t="s">
+      <c r="R33" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="R33" s="44">
+      <c r="S33" s="44">
         <v>30</v>
       </c>
-      <c r="S33" s="97" t="s">
+      <c r="T33" s="97" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P34" s="35" t="s">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q34" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="Q34" s="41" t="s">
+      <c r="R34" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="R34" s="44">
+      <c r="S34" s="44">
         <v>50</v>
       </c>
-      <c r="S34" s="97" t="s">
+      <c r="T34" s="97" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P35" s="35" t="s">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q35" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="Q35" s="41" t="s">
+      <c r="R35" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="R35" s="44">
+      <c r="S35" s="44">
         <v>20</v>
       </c>
-      <c r="S35" s="97" t="s">
+      <c r="T35" s="97" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P36" s="35" t="s">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q36" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="Q36" s="41" t="s">
+      <c r="R36" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="R36" s="44">
+      <c r="S36" s="44">
         <v>30</v>
       </c>
-      <c r="S36" s="97" t="s">
+      <c r="T36" s="97" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P37" s="36" t="s">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q37" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="Q37" s="42" t="s">
+      <c r="R37" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="R37" s="45" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="S37" s="98" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S37" s="45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T37" s="98" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="9"/>
-      <c r="P38" s="35" t="s">
+      <c r="Q38" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="Q38" s="39" t="s">
+      <c r="R38" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="R38" s="39">
+      <c r="S38" s="39">
         <v>50</v>
       </c>
-      <c r="S38" s="40" t="s">
+      <c r="T38" s="40" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="P39" s="35" t="s">
+      <c r="Q39" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="Q39" s="39" t="s">
+      <c r="R39" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="R39" s="39">
+      <c r="S39" s="39">
         <v>30</v>
       </c>
-      <c r="S39" s="40" t="s">
+      <c r="T39" s="40" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="9"/>
-      <c r="P40" s="36" t="s">
+      <c r="Q40" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="Q40" s="96" t="s">
+      <c r="R40" s="96" t="s">
         <v>130</v>
       </c>
-      <c r="R40" s="96" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="S40" s="43" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S40" s="96" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T40" s="43" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="9"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="9"/>
@@ -4722,7 +4765,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E14 P14" twoDigitTextYear="1"/>
+    <ignoredError sqref="E14 Q14" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -4731,9 +4774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A19AA3B-A7B0-864C-B5E4-F8D7A1F6D4E7}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5144,7 +5185,7 @@
       <c r="E23" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="F23" s="114"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" s="35" t="s">
@@ -5159,7 +5200,7 @@
       <c r="E24" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="F24" s="115"/>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" s="35" t="s">
@@ -5174,7 +5215,7 @@
       <c r="E25" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="F25" s="115"/>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B26" s="35" t="s">
@@ -5189,7 +5230,7 @@
       <c r="E26" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="115"/>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" s="35" t="s">
@@ -5204,7 +5245,7 @@
       <c r="E27" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="F27" s="115"/>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" s="36" t="s">
@@ -5219,7 +5260,7 @@
       <c r="E28" s="43" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F28" s="115"/>
+      <c r="F28" s="3"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="47" t="s">

</xml_diff>